<commit_message>
17 tabelas - uso em formulas
</commit_message>
<xml_diff>
--- a/005-formatacao/17-tabelas-usoEmFormulas.xlsx
+++ b/005-formatacao/17-tabelas-usoEmFormulas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joaof\Desktop\Excel Imp\Módulo 3 - Formatação\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jorge\Desktop\hashtag\hashtagExcel\005-formatacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3424B7D9-647F-4B3F-BFFA-FC4317AB10A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{176685D9-D491-4962-97D9-7826F1A39F4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{F1DCBCDB-AE2B-43B4-B740-43329A64DDA9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F1DCBCDB-AE2B-43B4-B740-43329A64DDA9}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="15">
   <si>
     <t>Vendedor</t>
   </si>
@@ -117,7 +117,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -128,11 +128,41 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="8">
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;R$&quot;\ #,##0.00"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;R$&quot;\ #,##0.00"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -145,8 +175,25 @@
 </styleSheet>
 </file>
 
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F96FE1AF-D7F3-4CBB-BB1C-A95F0EECB273}" name="Vendas" displayName="Vendas" ref="A1:F299" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+  <autoFilter ref="A1:F299" xr:uid="{F96FE1AF-D7F3-4CBB-BB1C-A95F0EECB273}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{E4D2512F-A84C-4FFF-A16F-787E601C8461}" name="Vendedor" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{645B0082-A677-4113-95A3-B972AF1995AA}" name="Produto" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{18C19413-ED02-4313-A9D6-EA9AC3E1495A}" name="Data" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{594A84F1-032F-4D5F-AB6F-319EEEDEA73F}" name="Qtd." dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{DAF8C70F-1BB2-4ABC-B47E-BBD4FB404C4A}" name="ValorProduto" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{B6B1D439-D71A-4C77-8AAD-D65B38FC6B65}" name="ValorTotal" dataDxfId="2">
+      <calculatedColumnFormula>E2*D2</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -442,20 +489,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B57C723-6BDD-4285-A449-C142A2C89BA1}">
-  <dimension ref="A1:F297"/>
+  <dimension ref="A1:H299"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="F299" sqref="F299"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="16.109375" customWidth="1"/>
-    <col min="4" max="4" width="7.77734375" customWidth="1"/>
-    <col min="5" max="6" width="16.109375" customWidth="1"/>
+    <col min="1" max="3" width="16.140625" customWidth="1"/>
+    <col min="4" max="4" width="7.7109375" customWidth="1"/>
+    <col min="5" max="6" width="16.140625" customWidth="1"/>
+    <col min="8" max="8" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -475,7 +523,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -495,8 +543,12 @@
         <f t="shared" ref="F2:F65" si="0">E2*D2</f>
         <v>119.69999999999999</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H2" s="4">
+        <f>SUM(F2:F297)</f>
+        <v>54889.20000000015</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -516,8 +568,12 @@
         <f t="shared" si="0"/>
         <v>421.20000000000005</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H3" s="4">
+        <f>SUM(F2:F299)</f>
+        <v>74914.200000000157</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -538,7 +594,7 @@
         <v>59.9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -559,7 +615,7 @@
         <v>421.20000000000005</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -579,8 +635,12 @@
         <f t="shared" si="0"/>
         <v>199.9</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H6" s="4">
+        <f>SUM(Vendas[ValorTotal])</f>
+        <v>74914.200000000157</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
@@ -601,7 +661,7 @@
         <v>199.9</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
@@ -622,7 +682,7 @@
         <v>59.9</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
@@ -643,7 +703,7 @@
         <v>119.8</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
@@ -664,7 +724,7 @@
         <v>127.5</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
@@ -685,7 +745,7 @@
         <v>399.8</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
@@ -706,7 +766,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
@@ -727,7 +787,7 @@
         <v>140.4</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
@@ -748,7 +808,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>6</v>
       </c>
@@ -769,7 +829,7 @@
         <v>280.8</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>11</v>
       </c>
@@ -790,7 +850,7 @@
         <v>79.8</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>8</v>
       </c>
@@ -811,7 +871,7 @@
         <v>39.9</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>6</v>
       </c>
@@ -832,7 +892,7 @@
         <v>39.9</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>6</v>
       </c>
@@ -853,7 +913,7 @@
         <v>59.9</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>6</v>
       </c>
@@ -874,7 +934,7 @@
         <v>140.4</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>11</v>
       </c>
@@ -895,7 +955,7 @@
         <v>59.9</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>6</v>
       </c>
@@ -916,7 +976,7 @@
         <v>199.9</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>13</v>
       </c>
@@ -937,7 +997,7 @@
         <v>421.20000000000005</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>8</v>
       </c>
@@ -958,7 +1018,7 @@
         <v>59.9</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>8</v>
       </c>
@@ -979,7 +1039,7 @@
         <v>599.70000000000005</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>11</v>
       </c>
@@ -1000,7 +1060,7 @@
         <v>280.8</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>13</v>
       </c>
@@ -1021,7 +1081,7 @@
         <v>119.8</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>8</v>
       </c>
@@ -1042,7 +1102,7 @@
         <v>140.4</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>13</v>
       </c>
@@ -1063,7 +1123,7 @@
         <v>140.4</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>13</v>
       </c>
@@ -1084,7 +1144,7 @@
         <v>199.9</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>6</v>
       </c>
@@ -1105,7 +1165,7 @@
         <v>382.5</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>11</v>
       </c>
@@ -1126,7 +1186,7 @@
         <v>127.5</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>6</v>
       </c>
@@ -1147,7 +1207,7 @@
         <v>399.8</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>11</v>
       </c>
@@ -1168,7 +1228,7 @@
         <v>59.9</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>8</v>
       </c>
@@ -1189,7 +1249,7 @@
         <v>127.5</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>13</v>
       </c>
@@ -1210,7 +1270,7 @@
         <v>59.9</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>13</v>
       </c>
@@ -1231,7 +1291,7 @@
         <v>119.69999999999999</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>8</v>
       </c>
@@ -1252,7 +1312,7 @@
         <v>79.8</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>13</v>
       </c>
@@ -1273,7 +1333,7 @@
         <v>199.9</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>6</v>
       </c>
@@ -1294,7 +1354,7 @@
         <v>140.4</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>11</v>
       </c>
@@ -1315,7 +1375,7 @@
         <v>59.9</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>6</v>
       </c>
@@ -1336,7 +1396,7 @@
         <v>127.5</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>8</v>
       </c>
@@ -1357,7 +1417,7 @@
         <v>127.5</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>13</v>
       </c>
@@ -1378,7 +1438,7 @@
         <v>119.8</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>11</v>
       </c>
@@ -1399,7 +1459,7 @@
         <v>39.9</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>6</v>
       </c>
@@ -1420,7 +1480,7 @@
         <v>127.5</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>11</v>
       </c>
@@ -1441,7 +1501,7 @@
         <v>119.8</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>13</v>
       </c>
@@ -1462,7 +1522,7 @@
         <v>199.9</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>8</v>
       </c>
@@ -1483,7 +1543,7 @@
         <v>127.5</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>13</v>
       </c>
@@ -1504,7 +1564,7 @@
         <v>382.5</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>8</v>
       </c>
@@ -1525,7 +1585,7 @@
         <v>140.4</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>13</v>
       </c>
@@ -1546,7 +1606,7 @@
         <v>59.9</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>13</v>
       </c>
@@ -1567,7 +1627,7 @@
         <v>421.20000000000005</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>11</v>
       </c>
@@ -1588,7 +1648,7 @@
         <v>119.69999999999999</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>11</v>
       </c>
@@ -1609,7 +1669,7 @@
         <v>119.8</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>8</v>
       </c>
@@ -1630,7 +1690,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>11</v>
       </c>
@@ -1651,7 +1711,7 @@
         <v>199.9</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>11</v>
       </c>
@@ -1672,7 +1732,7 @@
         <v>127.5</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>8</v>
       </c>
@@ -1693,7 +1753,7 @@
         <v>59.9</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>13</v>
       </c>
@@ -1714,7 +1774,7 @@
         <v>179.7</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>11</v>
       </c>
@@ -1735,7 +1795,7 @@
         <v>79.8</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>11</v>
       </c>
@@ -1756,7 +1816,7 @@
         <v>199.9</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>11</v>
       </c>
@@ -1777,7 +1837,7 @@
         <v>140.4</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>8</v>
       </c>
@@ -1798,7 +1858,7 @@
         <v>39.9</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>6</v>
       </c>
@@ -1819,7 +1879,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>6</v>
       </c>
@@ -1840,7 +1900,7 @@
         <v>199.9</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>6</v>
       </c>
@@ -1861,7 +1921,7 @@
         <v>79.8</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>13</v>
       </c>
@@ -1882,7 +1942,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>13</v>
       </c>
@@ -1903,7 +1963,7 @@
         <v>140.4</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>6</v>
       </c>
@@ -1924,7 +1984,7 @@
         <v>179.7</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>13</v>
       </c>
@@ -1945,7 +2005,7 @@
         <v>39.9</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>8</v>
       </c>
@@ -1966,7 +2026,7 @@
         <v>140.4</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>8</v>
       </c>
@@ -1987,7 +2047,7 @@
         <v>399.8</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>13</v>
       </c>
@@ -2008,7 +2068,7 @@
         <v>59.9</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>11</v>
       </c>
@@ -2029,7 +2089,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>6</v>
       </c>
@@ -2050,7 +2110,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>13</v>
       </c>
@@ -2071,7 +2131,7 @@
         <v>127.5</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>6</v>
       </c>
@@ -2092,7 +2152,7 @@
         <v>39.9</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>8</v>
       </c>
@@ -2113,7 +2173,7 @@
         <v>119.69999999999999</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>13</v>
       </c>
@@ -2134,7 +2194,7 @@
         <v>382.5</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>8</v>
       </c>
@@ -2155,7 +2215,7 @@
         <v>119.69999999999999</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>8</v>
       </c>
@@ -2176,7 +2236,7 @@
         <v>140.4</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>11</v>
       </c>
@@ -2197,7 +2257,7 @@
         <v>59.9</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>13</v>
       </c>
@@ -2218,7 +2278,7 @@
         <v>280.8</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>6</v>
       </c>
@@ -2239,7 +2299,7 @@
         <v>59.9</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>6</v>
       </c>
@@ -2260,7 +2320,7 @@
         <v>421.20000000000005</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>11</v>
       </c>
@@ -2281,7 +2341,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>6</v>
       </c>
@@ -2302,7 +2362,7 @@
         <v>127.5</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>8</v>
       </c>
@@ -2323,7 +2383,7 @@
         <v>199.9</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>8</v>
       </c>
@@ -2344,7 +2404,7 @@
         <v>119.8</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>11</v>
       </c>
@@ -2365,7 +2425,7 @@
         <v>599.70000000000005</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>13</v>
       </c>
@@ -2386,7 +2446,7 @@
         <v>179.7</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>8</v>
       </c>
@@ -2407,7 +2467,7 @@
         <v>119.69999999999999</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>13</v>
       </c>
@@ -2428,7 +2488,7 @@
         <v>199.9</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>13</v>
       </c>
@@ -2449,7 +2509,7 @@
         <v>127.5</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>13</v>
       </c>
@@ -2470,7 +2530,7 @@
         <v>140.4</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>8</v>
       </c>
@@ -2491,7 +2551,7 @@
         <v>140.4</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>6</v>
       </c>
@@ -2512,7 +2572,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>11</v>
       </c>
@@ -2533,7 +2593,7 @@
         <v>39.9</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>6</v>
       </c>
@@ -2554,7 +2614,7 @@
         <v>79.8</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>11</v>
       </c>
@@ -2575,7 +2635,7 @@
         <v>119.8</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>8</v>
       </c>
@@ -2596,7 +2656,7 @@
         <v>119.8</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>11</v>
       </c>
@@ -2617,7 +2677,7 @@
         <v>127.5</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>13</v>
       </c>
@@ -2638,7 +2698,7 @@
         <v>59.9</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>6</v>
       </c>
@@ -2659,7 +2719,7 @@
         <v>199.9</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>11</v>
       </c>
@@ -2680,7 +2740,7 @@
         <v>421.20000000000005</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>13</v>
       </c>
@@ -2701,7 +2761,7 @@
         <v>127.5</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>11</v>
       </c>
@@ -2722,7 +2782,7 @@
         <v>179.7</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>8</v>
       </c>
@@ -2743,7 +2803,7 @@
         <v>399.8</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>6</v>
       </c>
@@ -2764,7 +2824,7 @@
         <v>119.8</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>6</v>
       </c>
@@ -2785,7 +2845,7 @@
         <v>140.4</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>6</v>
       </c>
@@ -2806,7 +2866,7 @@
         <v>79.8</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>6</v>
       </c>
@@ -2827,7 +2887,7 @@
         <v>399.8</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
         <v>13</v>
       </c>
@@ -2848,7 +2908,7 @@
         <v>127.5</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>11</v>
       </c>
@@ -2869,7 +2929,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>11</v>
       </c>
@@ -2890,7 +2950,7 @@
         <v>421.20000000000005</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>8</v>
       </c>
@@ -2911,7 +2971,7 @@
         <v>127.5</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>6</v>
       </c>
@@ -2932,7 +2992,7 @@
         <v>59.9</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
         <v>6</v>
       </c>
@@ -2953,7 +3013,7 @@
         <v>140.4</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
         <v>8</v>
       </c>
@@ -2974,7 +3034,7 @@
         <v>59.9</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>6</v>
       </c>
@@ -2995,7 +3055,7 @@
         <v>39.9</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>11</v>
       </c>
@@ -3016,7 +3076,7 @@
         <v>199.9</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
         <v>6</v>
       </c>
@@ -3037,7 +3097,7 @@
         <v>127.5</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
         <v>8</v>
       </c>
@@ -3058,7 +3118,7 @@
         <v>140.4</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
         <v>13</v>
       </c>
@@ -3079,7 +3139,7 @@
         <v>199.9</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
         <v>13</v>
       </c>
@@ -3100,7 +3160,7 @@
         <v>59.9</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
         <v>6</v>
       </c>
@@ -3121,7 +3181,7 @@
         <v>140.4</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
         <v>13</v>
       </c>
@@ -3142,7 +3202,7 @@
         <v>179.7</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
         <v>8</v>
       </c>
@@ -3163,7 +3223,7 @@
         <v>39.9</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
         <v>13</v>
       </c>
@@ -3184,7 +3244,7 @@
         <v>399.8</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
         <v>11</v>
       </c>
@@ -3205,7 +3265,7 @@
         <v>199.9</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
         <v>11</v>
       </c>
@@ -3226,7 +3286,7 @@
         <v>140.4</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
         <v>6</v>
       </c>
@@ -3247,7 +3307,7 @@
         <v>119.69999999999999</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
         <v>6</v>
       </c>
@@ -3268,7 +3328,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
         <v>6</v>
       </c>
@@ -3289,7 +3349,7 @@
         <v>119.8</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
         <v>11</v>
       </c>
@@ -3310,7 +3370,7 @@
         <v>382.5</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
         <v>11</v>
       </c>
@@ -3331,7 +3391,7 @@
         <v>39.9</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
         <v>13</v>
       </c>
@@ -3352,7 +3412,7 @@
         <v>127.5</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
         <v>8</v>
       </c>
@@ -3373,7 +3433,7 @@
         <v>127.5</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
         <v>11</v>
       </c>
@@ -3394,7 +3454,7 @@
         <v>199.9</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
         <v>6</v>
       </c>
@@ -3415,7 +3475,7 @@
         <v>199.9</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
         <v>6</v>
       </c>
@@ -3436,7 +3496,7 @@
         <v>127.5</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
         <v>8</v>
       </c>
@@ -3457,7 +3517,7 @@
         <v>39.9</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
         <v>11</v>
       </c>
@@ -3478,7 +3538,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
         <v>8</v>
       </c>
@@ -3499,7 +3559,7 @@
         <v>119.8</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
         <v>13</v>
       </c>
@@ -3520,7 +3580,7 @@
         <v>59.9</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
         <v>11</v>
       </c>
@@ -3541,7 +3601,7 @@
         <v>59.9</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
         <v>8</v>
       </c>
@@ -3562,7 +3622,7 @@
         <v>421.20000000000005</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
         <v>6</v>
       </c>
@@ -3583,7 +3643,7 @@
         <v>59.9</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
         <v>13</v>
       </c>
@@ -3604,7 +3664,7 @@
         <v>179.7</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
         <v>13</v>
       </c>
@@ -3625,7 +3685,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
         <v>8</v>
       </c>
@@ -3646,7 +3706,7 @@
         <v>599.70000000000005</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
         <v>13</v>
       </c>
@@ -3667,7 +3727,7 @@
         <v>399.8</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
         <v>13</v>
       </c>
@@ -3688,7 +3748,7 @@
         <v>140.4</v>
       </c>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
         <v>11</v>
       </c>
@@ -3709,7 +3769,7 @@
         <v>79.8</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
         <v>11</v>
       </c>
@@ -3730,7 +3790,7 @@
         <v>421.20000000000005</v>
       </c>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
         <v>8</v>
       </c>
@@ -3751,7 +3811,7 @@
         <v>59.9</v>
       </c>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
         <v>6</v>
       </c>
@@ -3772,7 +3832,7 @@
         <v>127.5</v>
       </c>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
         <v>11</v>
       </c>
@@ -3793,7 +3853,7 @@
         <v>79.8</v>
       </c>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
         <v>6</v>
       </c>
@@ -3814,7 +3874,7 @@
         <v>59.9</v>
       </c>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
         <v>11</v>
       </c>
@@ -3835,7 +3895,7 @@
         <v>599.70000000000005</v>
       </c>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
         <v>11</v>
       </c>
@@ -3856,7 +3916,7 @@
         <v>59.9</v>
       </c>
     </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
         <v>13</v>
       </c>
@@ -3877,7 +3937,7 @@
         <v>140.4</v>
       </c>
     </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
         <v>8</v>
       </c>
@@ -3898,7 +3958,7 @@
         <v>39.9</v>
       </c>
     </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
         <v>8</v>
       </c>
@@ -3919,7 +3979,7 @@
         <v>59.9</v>
       </c>
     </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
         <v>6</v>
       </c>
@@ -3940,7 +4000,7 @@
         <v>199.9</v>
       </c>
     </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
         <v>11</v>
       </c>
@@ -3961,7 +4021,7 @@
         <v>127.5</v>
       </c>
     </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
         <v>13</v>
       </c>
@@ -3982,7 +4042,7 @@
         <v>199.9</v>
       </c>
     </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
         <v>8</v>
       </c>
@@ -4003,7 +4063,7 @@
         <v>382.5</v>
       </c>
     </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
         <v>6</v>
       </c>
@@ -4024,7 +4084,7 @@
         <v>199.9</v>
       </c>
     </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A171" s="1" t="s">
         <v>8</v>
       </c>
@@ -4045,7 +4105,7 @@
         <v>39.9</v>
       </c>
     </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A172" s="1" t="s">
         <v>11</v>
       </c>
@@ -4066,7 +4126,7 @@
         <v>399.8</v>
       </c>
     </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A173" s="1" t="s">
         <v>6</v>
       </c>
@@ -4087,7 +4147,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="s">
         <v>11</v>
       </c>
@@ -4108,7 +4168,7 @@
         <v>140.4</v>
       </c>
     </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A175" s="1" t="s">
         <v>8</v>
       </c>
@@ -4129,7 +4189,7 @@
         <v>140.4</v>
       </c>
     </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="s">
         <v>13</v>
       </c>
@@ -4150,7 +4210,7 @@
         <v>599.70000000000005</v>
       </c>
     </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A177" s="1" t="s">
         <v>8</v>
       </c>
@@ -4171,7 +4231,7 @@
         <v>127.5</v>
       </c>
     </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A178" s="1" t="s">
         <v>11</v>
       </c>
@@ -4192,7 +4252,7 @@
         <v>59.9</v>
       </c>
     </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A179" s="1" t="s">
         <v>6</v>
       </c>
@@ -4213,7 +4273,7 @@
         <v>421.20000000000005</v>
       </c>
     </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A180" s="1" t="s">
         <v>13</v>
       </c>
@@ -4234,7 +4294,7 @@
         <v>39.9</v>
       </c>
     </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A181" s="1" t="s">
         <v>6</v>
       </c>
@@ -4255,7 +4315,7 @@
         <v>59.9</v>
       </c>
     </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A182" s="1" t="s">
         <v>8</v>
       </c>
@@ -4276,7 +4336,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A183" s="1" t="s">
         <v>8</v>
       </c>
@@ -4297,7 +4357,7 @@
         <v>39.9</v>
       </c>
     </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A184" s="1" t="s">
         <v>8</v>
       </c>
@@ -4318,7 +4378,7 @@
         <v>399.8</v>
       </c>
     </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A185" s="1" t="s">
         <v>6</v>
       </c>
@@ -4339,7 +4399,7 @@
         <v>79.8</v>
       </c>
     </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A186" s="1" t="s">
         <v>6</v>
       </c>
@@ -4360,7 +4420,7 @@
         <v>421.20000000000005</v>
       </c>
     </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A187" s="1" t="s">
         <v>11</v>
       </c>
@@ -4381,7 +4441,7 @@
         <v>127.5</v>
       </c>
     </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A188" s="1" t="s">
         <v>11</v>
       </c>
@@ -4402,7 +4462,7 @@
         <v>599.70000000000005</v>
       </c>
     </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A189" s="1" t="s">
         <v>8</v>
       </c>
@@ -4423,7 +4483,7 @@
         <v>421.20000000000005</v>
       </c>
     </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A190" s="1" t="s">
         <v>6</v>
       </c>
@@ -4444,7 +4504,7 @@
         <v>59.9</v>
       </c>
     </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A191" s="1" t="s">
         <v>11</v>
       </c>
@@ -4465,7 +4525,7 @@
         <v>421.20000000000005</v>
       </c>
     </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A192" s="1" t="s">
         <v>8</v>
       </c>
@@ -4486,7 +4546,7 @@
         <v>140.4</v>
       </c>
     </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A193" s="1" t="s">
         <v>8</v>
       </c>
@@ -4507,7 +4567,7 @@
         <v>59.9</v>
       </c>
     </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A194" s="1" t="s">
         <v>6</v>
       </c>
@@ -4528,7 +4588,7 @@
         <v>280.8</v>
       </c>
     </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A195" s="1" t="s">
         <v>13</v>
       </c>
@@ -4549,7 +4609,7 @@
         <v>39.9</v>
       </c>
     </row>
-    <row r="196" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A196" s="1" t="s">
         <v>11</v>
       </c>
@@ -4570,7 +4630,7 @@
         <v>127.5</v>
       </c>
     </row>
-    <row r="197" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A197" s="1" t="s">
         <v>11</v>
       </c>
@@ -4591,7 +4651,7 @@
         <v>39.9</v>
       </c>
     </row>
-    <row r="198" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A198" s="1" t="s">
         <v>13</v>
       </c>
@@ -4612,7 +4672,7 @@
         <v>59.9</v>
       </c>
     </row>
-    <row r="199" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A199" s="1" t="s">
         <v>11</v>
       </c>
@@ -4633,7 +4693,7 @@
         <v>199.9</v>
       </c>
     </row>
-    <row r="200" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A200" s="1" t="s">
         <v>13</v>
       </c>
@@ -4654,7 +4714,7 @@
         <v>382.5</v>
       </c>
     </row>
-    <row r="201" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A201" s="1" t="s">
         <v>8</v>
       </c>
@@ -4675,7 +4735,7 @@
         <v>199.9</v>
       </c>
     </row>
-    <row r="202" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A202" s="1" t="s">
         <v>11</v>
       </c>
@@ -4696,7 +4756,7 @@
         <v>59.9</v>
       </c>
     </row>
-    <row r="203" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A203" s="1" t="s">
         <v>6</v>
       </c>
@@ -4717,7 +4777,7 @@
         <v>59.9</v>
       </c>
     </row>
-    <row r="204" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A204" s="1" t="s">
         <v>13</v>
       </c>
@@ -4738,7 +4798,7 @@
         <v>199.9</v>
       </c>
     </row>
-    <row r="205" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A205" s="1" t="s">
         <v>13</v>
       </c>
@@ -4759,7 +4819,7 @@
         <v>39.9</v>
       </c>
     </row>
-    <row r="206" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A206" s="1" t="s">
         <v>6</v>
       </c>
@@ -4780,7 +4840,7 @@
         <v>399.8</v>
       </c>
     </row>
-    <row r="207" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A207" s="1" t="s">
         <v>8</v>
       </c>
@@ -4801,7 +4861,7 @@
         <v>199.9</v>
       </c>
     </row>
-    <row r="208" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A208" s="1" t="s">
         <v>8</v>
       </c>
@@ -4822,7 +4882,7 @@
         <v>39.9</v>
       </c>
     </row>
-    <row r="209" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A209" s="1" t="s">
         <v>13</v>
       </c>
@@ -4843,7 +4903,7 @@
         <v>140.4</v>
       </c>
     </row>
-    <row r="210" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A210" s="1" t="s">
         <v>6</v>
       </c>
@@ -4864,7 +4924,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="211" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A211" s="1" t="s">
         <v>11</v>
       </c>
@@ -4885,7 +4945,7 @@
         <v>59.9</v>
       </c>
     </row>
-    <row r="212" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A212" s="1" t="s">
         <v>6</v>
       </c>
@@ -4906,7 +4966,7 @@
         <v>140.4</v>
       </c>
     </row>
-    <row r="213" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A213" s="1" t="s">
         <v>11</v>
       </c>
@@ -4927,7 +4987,7 @@
         <v>127.5</v>
       </c>
     </row>
-    <row r="214" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A214" s="1" t="s">
         <v>13</v>
       </c>
@@ -4948,7 +5008,7 @@
         <v>127.5</v>
       </c>
     </row>
-    <row r="215" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A215" s="1" t="s">
         <v>11</v>
       </c>
@@ -4969,7 +5029,7 @@
         <v>599.70000000000005</v>
       </c>
     </row>
-    <row r="216" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A216" s="1" t="s">
         <v>8</v>
       </c>
@@ -4990,7 +5050,7 @@
         <v>140.4</v>
       </c>
     </row>
-    <row r="217" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A217" s="1" t="s">
         <v>6</v>
       </c>
@@ -5011,7 +5071,7 @@
         <v>140.4</v>
       </c>
     </row>
-    <row r="218" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A218" s="1" t="s">
         <v>8</v>
       </c>
@@ -5032,7 +5092,7 @@
         <v>382.5</v>
       </c>
     </row>
-    <row r="219" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A219" s="1" t="s">
         <v>13</v>
       </c>
@@ -5053,7 +5113,7 @@
         <v>39.9</v>
       </c>
     </row>
-    <row r="220" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A220" s="1" t="s">
         <v>8</v>
       </c>
@@ -5074,7 +5134,7 @@
         <v>59.9</v>
       </c>
     </row>
-    <row r="221" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A221" s="1" t="s">
         <v>11</v>
       </c>
@@ -5095,7 +5155,7 @@
         <v>399.8</v>
       </c>
     </row>
-    <row r="222" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A222" s="1" t="s">
         <v>6</v>
       </c>
@@ -5116,7 +5176,7 @@
         <v>39.9</v>
       </c>
     </row>
-    <row r="223" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A223" s="1" t="s">
         <v>8</v>
       </c>
@@ -5137,7 +5197,7 @@
         <v>280.8</v>
       </c>
     </row>
-    <row r="224" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A224" s="1" t="s">
         <v>11</v>
       </c>
@@ -5158,7 +5218,7 @@
         <v>382.5</v>
       </c>
     </row>
-    <row r="225" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A225" s="1" t="s">
         <v>11</v>
       </c>
@@ -5179,7 +5239,7 @@
         <v>39.9</v>
       </c>
     </row>
-    <row r="226" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A226" s="1" t="s">
         <v>11</v>
       </c>
@@ -5200,7 +5260,7 @@
         <v>59.9</v>
       </c>
     </row>
-    <row r="227" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A227" s="1" t="s">
         <v>13</v>
       </c>
@@ -5221,7 +5281,7 @@
         <v>140.4</v>
       </c>
     </row>
-    <row r="228" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A228" s="1" t="s">
         <v>8</v>
       </c>
@@ -5242,7 +5302,7 @@
         <v>199.9</v>
       </c>
     </row>
-    <row r="229" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A229" s="1" t="s">
         <v>8</v>
       </c>
@@ -5263,7 +5323,7 @@
         <v>199.9</v>
       </c>
     </row>
-    <row r="230" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A230" s="1" t="s">
         <v>11</v>
       </c>
@@ -5284,7 +5344,7 @@
         <v>421.20000000000005</v>
       </c>
     </row>
-    <row r="231" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A231" s="1" t="s">
         <v>8</v>
       </c>
@@ -5305,7 +5365,7 @@
         <v>140.4</v>
       </c>
     </row>
-    <row r="232" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A232" s="1" t="s">
         <v>11</v>
       </c>
@@ -5326,7 +5386,7 @@
         <v>127.5</v>
       </c>
     </row>
-    <row r="233" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A233" s="1" t="s">
         <v>6</v>
       </c>
@@ -5347,7 +5407,7 @@
         <v>599.70000000000005</v>
       </c>
     </row>
-    <row r="234" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A234" s="1" t="s">
         <v>11</v>
       </c>
@@ -5368,7 +5428,7 @@
         <v>199.9</v>
       </c>
     </row>
-    <row r="235" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A235" s="1" t="s">
         <v>6</v>
       </c>
@@ -5389,7 +5449,7 @@
         <v>127.5</v>
       </c>
     </row>
-    <row r="236" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A236" s="1" t="s">
         <v>11</v>
       </c>
@@ -5410,7 +5470,7 @@
         <v>39.9</v>
       </c>
     </row>
-    <row r="237" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A237" s="1" t="s">
         <v>6</v>
       </c>
@@ -5431,7 +5491,7 @@
         <v>140.4</v>
       </c>
     </row>
-    <row r="238" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A238" s="1" t="s">
         <v>8</v>
       </c>
@@ -5452,7 +5512,7 @@
         <v>199.9</v>
       </c>
     </row>
-    <row r="239" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A239" s="1" t="s">
         <v>11</v>
       </c>
@@ -5473,7 +5533,7 @@
         <v>127.5</v>
       </c>
     </row>
-    <row r="240" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A240" s="1" t="s">
         <v>13</v>
       </c>
@@ -5494,7 +5554,7 @@
         <v>199.9</v>
       </c>
     </row>
-    <row r="241" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A241" s="1" t="s">
         <v>13</v>
       </c>
@@ -5515,7 +5575,7 @@
         <v>382.5</v>
       </c>
     </row>
-    <row r="242" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A242" s="1" t="s">
         <v>6</v>
       </c>
@@ -5536,7 +5596,7 @@
         <v>39.9</v>
       </c>
     </row>
-    <row r="243" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A243" s="1" t="s">
         <v>6</v>
       </c>
@@ -5557,7 +5617,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="244" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A244" s="1" t="s">
         <v>6</v>
       </c>
@@ -5578,7 +5638,7 @@
         <v>199.9</v>
       </c>
     </row>
-    <row r="245" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A245" s="1" t="s">
         <v>8</v>
       </c>
@@ -5599,7 +5659,7 @@
         <v>39.9</v>
       </c>
     </row>
-    <row r="246" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A246" s="1" t="s">
         <v>6</v>
       </c>
@@ -5620,7 +5680,7 @@
         <v>140.4</v>
       </c>
     </row>
-    <row r="247" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A247" s="1" t="s">
         <v>8</v>
       </c>
@@ -5641,7 +5701,7 @@
         <v>382.5</v>
       </c>
     </row>
-    <row r="248" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A248" s="1" t="s">
         <v>6</v>
       </c>
@@ -5662,7 +5722,7 @@
         <v>299.5</v>
       </c>
     </row>
-    <row r="249" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A249" s="1" t="s">
         <v>6</v>
       </c>
@@ -5683,7 +5743,7 @@
         <v>119.69999999999999</v>
       </c>
     </row>
-    <row r="250" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A250" s="1" t="s">
         <v>13</v>
       </c>
@@ -5704,7 +5764,7 @@
         <v>199.9</v>
       </c>
     </row>
-    <row r="251" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A251" s="1" t="s">
         <v>13</v>
       </c>
@@ -5725,7 +5785,7 @@
         <v>119.8</v>
       </c>
     </row>
-    <row r="252" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A252" s="1" t="s">
         <v>6</v>
       </c>
@@ -5746,7 +5806,7 @@
         <v>59.9</v>
       </c>
     </row>
-    <row r="253" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A253" s="1" t="s">
         <v>8</v>
       </c>
@@ -5767,7 +5827,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="254" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A254" s="1" t="s">
         <v>11</v>
       </c>
@@ -5788,7 +5848,7 @@
         <v>140.4</v>
       </c>
     </row>
-    <row r="255" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A255" s="1" t="s">
         <v>13</v>
       </c>
@@ -5809,7 +5869,7 @@
         <v>140.4</v>
       </c>
     </row>
-    <row r="256" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A256" s="1" t="s">
         <v>8</v>
       </c>
@@ -5830,7 +5890,7 @@
         <v>140.4</v>
       </c>
     </row>
-    <row r="257" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A257" s="1" t="s">
         <v>11</v>
       </c>
@@ -5851,7 +5911,7 @@
         <v>127.5</v>
       </c>
     </row>
-    <row r="258" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A258" s="1" t="s">
         <v>8</v>
       </c>
@@ -5868,11 +5928,11 @@
         <v>199.9</v>
       </c>
       <c r="F258" s="3">
-        <f t="shared" ref="F258:F297" si="4">E258*D258</f>
-        <v>199.9</v>
-      </c>
-    </row>
-    <row r="259" spans="1:6" x14ac:dyDescent="0.3">
+        <f t="shared" ref="F258:F298" si="4">E258*D258</f>
+        <v>199.9</v>
+      </c>
+    </row>
+    <row r="259" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A259" s="1" t="s">
         <v>6</v>
       </c>
@@ -5893,7 +5953,7 @@
         <v>599.70000000000005</v>
       </c>
     </row>
-    <row r="260" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A260" s="1" t="s">
         <v>6</v>
       </c>
@@ -5914,7 +5974,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="261" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A261" s="1" t="s">
         <v>8</v>
       </c>
@@ -5935,7 +5995,7 @@
         <v>399.8</v>
       </c>
     </row>
-    <row r="262" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A262" s="1" t="s">
         <v>11</v>
       </c>
@@ -5956,7 +6016,7 @@
         <v>280.8</v>
       </c>
     </row>
-    <row r="263" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A263" s="1" t="s">
         <v>11</v>
       </c>
@@ -5977,7 +6037,7 @@
         <v>39.9</v>
       </c>
     </row>
-    <row r="264" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A264" s="1" t="s">
         <v>8</v>
       </c>
@@ -5998,7 +6058,7 @@
         <v>59.9</v>
       </c>
     </row>
-    <row r="265" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A265" s="1" t="s">
         <v>6</v>
       </c>
@@ -6019,7 +6079,7 @@
         <v>140.4</v>
       </c>
     </row>
-    <row r="266" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A266" s="1" t="s">
         <v>6</v>
       </c>
@@ -6040,7 +6100,7 @@
         <v>59.9</v>
       </c>
     </row>
-    <row r="267" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A267" s="1" t="s">
         <v>6</v>
       </c>
@@ -6061,7 +6121,7 @@
         <v>399.8</v>
       </c>
     </row>
-    <row r="268" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A268" s="1" t="s">
         <v>13</v>
       </c>
@@ -6082,7 +6142,7 @@
         <v>421.20000000000005</v>
       </c>
     </row>
-    <row r="269" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A269" s="1" t="s">
         <v>6</v>
       </c>
@@ -6103,7 +6163,7 @@
         <v>127.5</v>
       </c>
     </row>
-    <row r="270" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A270" s="1" t="s">
         <v>6</v>
       </c>
@@ -6124,7 +6184,7 @@
         <v>140.4</v>
       </c>
     </row>
-    <row r="271" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A271" s="1" t="s">
         <v>8</v>
       </c>
@@ -6145,7 +6205,7 @@
         <v>39.9</v>
       </c>
     </row>
-    <row r="272" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A272" s="1" t="s">
         <v>13</v>
       </c>
@@ -6166,7 +6226,7 @@
         <v>199.9</v>
       </c>
     </row>
-    <row r="273" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A273" s="1" t="s">
         <v>13</v>
       </c>
@@ -6187,7 +6247,7 @@
         <v>59.9</v>
       </c>
     </row>
-    <row r="274" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A274" s="1" t="s">
         <v>13</v>
       </c>
@@ -6208,7 +6268,7 @@
         <v>140.4</v>
       </c>
     </row>
-    <row r="275" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A275" s="1" t="s">
         <v>8</v>
       </c>
@@ -6229,7 +6289,7 @@
         <v>179.7</v>
       </c>
     </row>
-    <row r="276" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A276" s="1" t="s">
         <v>8</v>
       </c>
@@ -6250,7 +6310,7 @@
         <v>199.9</v>
       </c>
     </row>
-    <row r="277" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A277" s="1" t="s">
         <v>11</v>
       </c>
@@ -6271,7 +6331,7 @@
         <v>39.9</v>
       </c>
     </row>
-    <row r="278" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A278" s="1" t="s">
         <v>13</v>
       </c>
@@ -6292,7 +6352,7 @@
         <v>199.9</v>
       </c>
     </row>
-    <row r="279" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A279" s="1" t="s">
         <v>11</v>
       </c>
@@ -6313,7 +6373,7 @@
         <v>39.9</v>
       </c>
     </row>
-    <row r="280" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A280" s="1" t="s">
         <v>11</v>
       </c>
@@ -6334,7 +6394,7 @@
         <v>399.8</v>
       </c>
     </row>
-    <row r="281" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A281" s="1" t="s">
         <v>13</v>
       </c>
@@ -6355,7 +6415,7 @@
         <v>119.8</v>
       </c>
     </row>
-    <row r="282" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A282" s="1" t="s">
         <v>8</v>
       </c>
@@ -6376,7 +6436,7 @@
         <v>39.9</v>
       </c>
     </row>
-    <row r="283" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A283" s="1" t="s">
         <v>13</v>
       </c>
@@ -6397,7 +6457,7 @@
         <v>140.4</v>
       </c>
     </row>
-    <row r="284" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A284" s="1" t="s">
         <v>8</v>
       </c>
@@ -6418,7 +6478,7 @@
         <v>179.7</v>
       </c>
     </row>
-    <row r="285" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A285" s="1" t="s">
         <v>6</v>
       </c>
@@ -6439,7 +6499,7 @@
         <v>39.9</v>
       </c>
     </row>
-    <row r="286" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A286" s="1" t="s">
         <v>11</v>
       </c>
@@ -6460,7 +6520,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="287" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A287" s="1" t="s">
         <v>11</v>
       </c>
@@ -6481,7 +6541,7 @@
         <v>140.4</v>
       </c>
     </row>
-    <row r="288" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A288" s="1" t="s">
         <v>6</v>
       </c>
@@ -6502,7 +6562,7 @@
         <v>127.5</v>
       </c>
     </row>
-    <row r="289" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A289" s="1" t="s">
         <v>8</v>
       </c>
@@ -6523,7 +6583,7 @@
         <v>39.9</v>
       </c>
     </row>
-    <row r="290" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A290" s="1" t="s">
         <v>13</v>
       </c>
@@ -6544,7 +6604,7 @@
         <v>119.8</v>
       </c>
     </row>
-    <row r="291" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A291" s="1" t="s">
         <v>11</v>
       </c>
@@ -6565,7 +6625,7 @@
         <v>39.9</v>
       </c>
     </row>
-    <row r="292" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A292" s="1" t="s">
         <v>8</v>
       </c>
@@ -6586,7 +6646,7 @@
         <v>59.9</v>
       </c>
     </row>
-    <row r="293" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A293" s="1" t="s">
         <v>6</v>
       </c>
@@ -6607,7 +6667,7 @@
         <v>599.70000000000005</v>
       </c>
     </row>
-    <row r="294" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A294" s="1" t="s">
         <v>6</v>
       </c>
@@ -6628,7 +6688,7 @@
         <v>59.9</v>
       </c>
     </row>
-    <row r="295" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A295" s="1" t="s">
         <v>11</v>
       </c>
@@ -6649,7 +6709,7 @@
         <v>382.5</v>
       </c>
     </row>
-    <row r="296" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A296" s="1" t="s">
         <v>8</v>
       </c>
@@ -6670,7 +6730,7 @@
         <v>140.4</v>
       </c>
     </row>
-    <row r="297" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A297" s="1" t="s">
         <v>11</v>
       </c>
@@ -6691,7 +6751,52 @@
         <v>119.8</v>
       </c>
     </row>
+    <row r="298" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A298" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B298" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C298" s="5">
+        <v>44834</v>
+      </c>
+      <c r="D298" s="1">
+        <v>1</v>
+      </c>
+      <c r="E298" s="3">
+        <v>25</v>
+      </c>
+      <c r="F298" s="3">
+        <f>E298*D298</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="299" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A299" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B299" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C299" s="2">
+        <v>44834</v>
+      </c>
+      <c r="D299" s="1">
+        <v>2</v>
+      </c>
+      <c r="E299" s="3">
+        <v>10000</v>
+      </c>
+      <c r="F299" s="3">
+        <f>E299*D299</f>
+        <v>20000</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>